<commit_message>
Update RNA-seq data prep documentation
</commit_message>
<xml_diff>
--- a/nanni_maize_2022/documentation/RNAseq_data_prep.xlsx
+++ b/nanni_maize_2022/documentation/RNAseq_data_prep.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHARE\McIntyre_Lab\maize_ozone_FINAL\2018\PacBio\documentation\github_documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ufgi$/SHARE/McIntyre_Lab/maize_ozone_FINAL/2018/PacBio/documentation/github_documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B15E645-4178-481E-A8E1-85A2D0646A68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AF8CAD-76A5-784C-B357-687F220D8B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t xml:space="preserve">maize RNAseq </t>
   </si>
@@ -60,18 +60,156 @@
     <t>notes</t>
   </si>
   <si>
-    <t>prep read data</t>
-  </si>
-  <si>
-    <t>run cutadapt, bbmerge and fqsplitDups on original data</t>
-  </si>
-  <si>
-    <t>/ufrc/mcintyre/share/maize_ainsworth/scripts/run_cut_bbM_fqSplit_rnaseq_02amm.sbatch
-/ufrc/mcintyre/share/maize_ainsworth/scripts/run_cut_bbM_fqSplit_rnaseq_1st_novogene_lane.sbatch</t>
-  </si>
-  <si>
-    <t>bbM_50perc_read_length.py
+    <t>PROJ=/ufrc/mcintyre/share/mazie_ainsworth</t>
+  </si>
+  <si>
+    <t>cutadapt/2.1
+bbmap/38.44
+python/2.7.14
+$PROJ/scripts/
+bbM_50perc_read_length.py
 fastqSplitDups_2MAI.py</t>
+  </si>
+  <si>
+    <t>$PROJ/original_data/RNAseq/Plate3-4/*
+$PROJ/design_files/maize_rnaseq_design_file_noHeader.csv</t>
+  </si>
+  <si>
+    <t>Data prep for rapid genomics run
+cutadapt
+    trim illumina truseq adapters
+    default values for max error rate and min overlap
+    See Notes for sequences used
+bbmerge
+    basic bbmerge to combine overlapping R1-R2 reads
+    merges by overlap
+        ## pfilter=1 allows only perfect overlap
+        ## minOverlap = 25% of RL
+Drop reads that are less than 50% of starting readLength
+fqsplitDups on SE merged and PE unmerged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        -a "AGATCGGAAGAGCACACGTCTGAACTCCAGTCA;max_error_rate=0.1;min_overlap=3" \
+        -A "AGATCGGAAGAGCGTCGTGTAGGGAAAGAGTGT;max_error_rate=0.1;min_overlap=3" \
+SAMPLEID=${SAMPLE}_techRep${TR}</t>
+  </si>
+  <si>
+    <t>$PROJ/cutadapt/
+${SAMPLEID}_R1.fastq
+${SAMPLEID}_R2.fastq
+$PROJ/cutadapt_bbmerge/
+${SAMPLEID}_bbmerge_min${MIN}.fastq
+${SAMPLEID}_R1_unmerge_min${MIN}.fastq
+${SAMPLEID}_R2_unmerge_min${MIN}.fastq
+$PROJ/cutadapt_bbmerge_GE_50perc_RL/${SAMPLEID}_bbmerge_min${MIN}.fastq
+$PROJ/cutadapt_bbmerge_LESS_50perc_RL/${SAMPLEID}_bbmerge_min${MIN}.fastq
+THE ABOVE FILES ARE DELETED
+$PROJ/dataPrepLogs/
+${SAMPLEID}_dataPrep.log
+${SAMPLEID}_bbmerge_min${MIN}_read_sizes.txt
+${SAMPLEID}_bbmerge_min${MIN}_ihist.txt
+${SAMPLEID}_fqSplitDup_on_bberge_min${MIN}_summary.csv
+${SAMPLEID}_fqSplitDup_on_bbmerge_min${MIN}.log
+${SAMPLEID}_fqSplitDup_on_bbUnm_min${MIN}_summary.csv
+${SAMPLEID}_fqSplitDupon_bbUnm_min${MIN}.log
+$PROJ/cutadapt_bbmerge_fastqSplitDups/
+${SAMPLEID}_fqSplitDup_on_bbmerge_min${MIN}_table.tsv
+${SAMPLEID}_fqSplitDup_on_bbUnm_min${MIN}_table.tsv
+${SAMPLEID}_bbmerge_min${MIN}_distinct.fq
+${SAMPLEID}_bbmerge_min${MIN}_duplicate.fq
+${SAMPLEID}_bbmerge_min${MIN}_single_duplicate.fq
+${SAMPLEID}_bbmerge_min${MIN}_uniq.fq
+${SAMPLEID}_fqSplitDup_on_unmerge_min${MIN}_table.tsv
+${SAMPLEID}_R1_unmerge_min${MIN}_noEmpty_distinct.fq
+${SAMPLEID}_R1_unmerge_min${MIN}_noEmpty_duplicate.fq
+${SAMPLEID}_R1_unmerge_min${MIN}_noEmpty_single_duplicate.fq
+${SAMPLEID}_R1_unmerge_min${MIN}_noEmpty_uniq.fq
+${SAMPLEID}_R2_unmerge_min${MIN}_noEmpty_distinct.fq
+${SAMPLEID}_R2_unmerge_min${MIN}_noEmpty_duplicate.fq
+${SAMPLEID}_R2_unmerge_min${MIN}_noEmpty_single_duplicate.fq
+${SAMPLEID}_R2_unmerge_min${MIN}_noEmpty_uniq.fq
+${SAMPLEID}_R1_widow_min${MIN}_distinct.fq
+${SAMPLEID}_R1_widow_min${MIN}_duplicate.fq
+${SAMPLEID}_R1_widow_min${MIN}_single_duplicate.fq
+${SAMPLEID}_R1_widow_min${MIN}_uniq.fq
+${SAMPLEID}_R2_widow_min${MIN}_distinct.fq
+${SAMPLEID}_R2_widow_min${MIN}_duplicate.fq
+${SAMPLEID}_R2_widow_min${MIN}_single_duplicate.fq
+${SAMPLEID}_R2_widow_min${MIN}_uniq.fq</t>
+  </si>
+  <si>
+    <t>prep read data rapid genomics</t>
+  </si>
+  <si>
+    <t>prep read data novogene</t>
+  </si>
+  <si>
+    <t>Data prep for novogene run
+cutadapt
+    trim illumina truseq adapters
+    default values for max error rate and min overlap
+    See Notes for sequences used
+bbmerge
+    basic bbmerge to combine overlapping R1-R2 reads
+    merges by overlap
+        ## pfilter=1 allows only perfect overlap
+        ## minOverlap = 25% of RL
+Drop reads that are less than 50% of starting readLength
+fqsplitDups on SE merged and PE unmerged</t>
+  </si>
+  <si>
+    <t>/ufrc/mcintyre/share/maize_ainsworth/scripts/run_cut_bbM_fqSplit_rnaseq_1st_novogene_lane.sbatch</t>
+  </si>
+  <si>
+    <t>/ufrc/mcintyre/share/maize_ainsworth/scripts/run_cut_bbM_fqSplit_rnaseq_02amm.sbatch</t>
+  </si>
+  <si>
+    <t>$PROJ/cutadapt_NG1/
+${SAMPLEID}_R1.fastq
+${SAMPLEID}_R2.fastq
+$PROJ/cutadapt_bbmerge_NG1/
+${SAMPLEID}_bbmerge_min${MIN}.fastq
+${SAMPLEID}_R1_unmerge_min${MIN}.fastq
+${SAMPLEID}_R2_unmerge_min${MIN}.fastq
+$PROJ/cutadapt_bbmerge_NG1_GE_50perc_RL/${SAMPLEID}_bbmerge_min${MIN}.fastq
+$PROJ/cutadapt_bbmerge_NG1_LESS_50perc_RL/${SAMPLEID}_bbmerge_min${MIN}.fastq
+THE ABOVE FILES ARE DELETED
+$PROJ/dataPrepLogs_NG1/
+${SAMPLEID}_dataPrep.log
+${SAMPLEID}_bbmerge_min${MIN}_read_sizes.txt
+${SAMPLEID}_bbmerge_min${MIN}_ihist.txt
+${SAMPLEID}_fqSplitDup_on_bberge_min${MIN}_summary.csv
+${SAMPLEID}_fqSplitDup_on_bbmerge_min${MIN}.log
+${SAMPLEID}_fqSplitDup_on_bbUnm_min${MIN}_summary.csv
+${SAMPLEID}_fqSplitDupon_bbUnm_min${MIN}.log
+$PROJ/cutadapt_bbmerge_fastqSplitDups_NG1/
+${SAMPLEID}_fqSplitDup_on_bbmerge_min${MIN}_table.tsv
+${SAMPLEID}_fqSplitDup_on_bbUnm_min${MIN}_table.tsv
+${SAMPLEID}_bbmerge_min${MIN}_distinct.fq
+${SAMPLEID}_bbmerge_min${MIN}_duplicate.fq
+${SAMPLEID}_bbmerge_min${MIN}_single_duplicate.fq
+${SAMPLEID}_bbmerge_min${MIN}_uniq.fq
+${SAMPLEID}_fqSplitDup_on_unmerge_min${MIN}_table.tsv
+${SAMPLEID}_R1_unmerge_min${MIN}_noEmpty_distinct.fq
+${SAMPLEID}_R1_unmerge_min${MIN}_noEmpty_duplicate.fq
+${SAMPLEID}_R1_unmerge_min${MIN}_noEmpty_single_duplicate.fq
+${SAMPLEID}_R1_unmerge_min${MIN}_noEmpty_uniq.fq
+${SAMPLEID}_R2_unmerge_min${MIN}_noEmpty_distinct.fq
+${SAMPLEID}_R2_unmerge_min${MIN}_noEmpty_duplicate.fq
+${SAMPLEID}_R2_unmerge_min${MIN}_noEmpty_single_duplicate.fq
+${SAMPLEID}_R2_unmerge_min${MIN}_noEmpty_uniq.fq
+${SAMPLEID}_R1_widow_min${MIN}_distinct.fq
+${SAMPLEID}_R1_widow_min${MIN}_duplicate.fq
+${SAMPLEID}_R1_widow_min${MIN}_single_duplicate.fq
+${SAMPLEID}_R1_widow_min${MIN}_uniq.fq
+${SAMPLEID}_R2_widow_min${MIN}_distinct.fq
+${SAMPLEID}_R2_widow_min${MIN}_duplicate.fq
+${SAMPLEID}_R2_widow_min${MIN}_single_duplicate.fq
+${SAMPLEID}_R2_widow_min${MIN}_uniq.fq</t>
+  </si>
+  <si>
+    <t>$PROJ/unzipped_FQ_RNAseq_novogene_1st_lane/*
+$PROJ/design_files/maize_rnaseq_design_file_noHeader.csv</t>
   </si>
 </sst>
 </file>
@@ -120,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -134,6 +272,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -452,44 +593,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="23.21875" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="46.5" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="43.44140625" customWidth="1"/>
-    <col min="7" max="7" width="46.5546875" customWidth="1"/>
+    <col min="6" max="6" width="43.5" customWidth="1"/>
+    <col min="7" max="7" width="56.5" customWidth="1"/>
+    <col min="9" max="9" width="90.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="8" spans="2:9" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -515,62 +660,93 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:9" s="6" customFormat="1" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="2:9" s="6" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="E10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="2:9" s="6" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="23" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="33" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="34" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="35" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="36" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="37" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="38" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="39" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="40" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="41" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="42" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="43" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="44" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="45" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="46" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>